<commit_message>
fix: Update font style for bottom sheet values in generate_excel function
</commit_message>
<xml_diff>
--- a/filestemplate/f1-buttom.xlsx
+++ b/filestemplate/f1-buttom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nattawutr./dormitory-management-information-system-ocr-engine/filestemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843142E0-C3D7-8B45-A6EA-1F550262729D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A399EDB2-4CE1-7743-8491-0083B905D8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="13160" windowWidth="21600" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,12 +467,87 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -512,85 +587,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -930,7 +930,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.35"/>
@@ -938,10 +938,10 @@
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" customWidth="1"/>
     <col min="3" max="3" width="3.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="4.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="5.83203125" style="1" customWidth="1"/>
@@ -957,15 +957,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
       <c r="H1" s="59"/>
       <c r="I1" s="59"/>
       <c r="J1" s="59"/>
@@ -982,18 +982,18 @@
     </row>
     <row r="3" spans="1:18" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G3" s="5"/>
-      <c r="I3" s="25" t="str">
+      <c r="I3" s="50" t="str">
         <f>BAHTTEXT(900)</f>
         <v>เก้าร้อยบาทถ้วน</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="27"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="52"/>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -1007,15 +1007,15 @@
         <v>3</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="55"/>
     </row>
     <row r="5" spans="1:18" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
@@ -1026,25 +1026,25 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="33"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="58"/>
     </row>
     <row r="6" spans="1:18" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1058,69 +1058,69 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:18" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="41" t="s">
+      <c r="G7" s="40"/>
+      <c r="H7" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="22" t="s">
+      <c r="I7" s="38"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="23" t="s">
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="24"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="49"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="34" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="35" t="s">
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>1</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="44"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="7"/>
       <c r="G9" s="9"/>
       <c r="H9" s="8"/>
@@ -1136,30 +1136,30 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="10"/>
       <c r="N10" s="11"/>
       <c r="Q10" s="11"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="12"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
@@ -1169,13 +1169,13 @@
       <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F12" s="55" t="s">
+      <c r="F12" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
@@ -1185,27 +1185,27 @@
       <c r="Q12" s="16"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="53" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="53"/>
-      <c r="P14" s="53"/>
-      <c r="Q14" s="53"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D15" s="17"/>
@@ -1220,29 +1220,45 @@
       </c>
     </row>
     <row r="18" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F18" s="51" t="s">
+      <c r="F18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
     </row>
     <row r="19" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="I3:Q5"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
     <mergeCell ref="F18:L18"/>
     <mergeCell ref="F19:L19"/>
     <mergeCell ref="H10:J10"/>
@@ -1251,22 +1267,6 @@
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H14:Q14"/>
     <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="I3:Q5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>